<commit_message>
new version 0.2 of the controlled vocabulary on the government document types. The owlVersionInfo property of the vocabulary explains in detail the changes that were applied. The readme reports the structure of the vocabulary in its version 0.1 and the changes in version 0.2
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-documents/government-documents-types/government-documents-types.xlsx
+++ b/VocabolariControllati/classifications-for-documents/government-documents-types/government-documents-types.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Dropbox/OntoPiA/DocumentiComuni/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Desktop/AGID/NuovoDATIGOV/DAF/Git/OntologieVocabolariControllati/VocabolariControllati/classifications-for-documents/government-documents-types/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88A9DDF4-8501-D04F-BDA7-948714BF322D}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BD022B-2132-2F41-AA3D-FEC818248152}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{211D512B-4A7E-2C48-891F-47DA42C0E5D3}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{211D512B-4A7E-2C48-891F-47DA42C0E5D3}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
   <si>
     <t>Documenti albo pretorio</t>
   </si>
@@ -89,18 +89,12 @@
     <t>Documenti (tecnici) di supprto</t>
   </si>
   <si>
-    <t>Rientrano in questo concetto tutti i documenti relativi al funzionamento interno come per esempio rendimenti, rendiconti, procedure, bilanci consuntivi e preventivi</t>
-  </si>
-  <si>
     <t>Rientrano in questo concetto l'insieme dei moduli in uso presso gli uffici della pubblica amministrazione. Esempi includono, modulo primario,  moduli allegati, ecc.</t>
   </si>
   <si>
     <t>Rientrano in questo concetto tutti quei documenti che devono essere pubblicati nell'albo pretorio nel caso di amministrazioni comunali. Tale concetto è oggetto a sua volta di un vocabolario controllato dedicato già disponibile a questo URI https://w3id.org/italia/controlled-vocabulary/municipal-board-notice</t>
   </si>
   <si>
-    <t>Rientrano in questo concetto tutte le tipologie di atti normativi quali per esempio la costituzione, il decreto legislativo, il decreto legge, il decreto reale, il regio decreto ecc.</t>
-  </si>
-  <si>
     <t>In questa concetto si possono ricomprendere tutti quei documenti che consentono di instaurare un rapporto di collaborazione tra enti. Esempi includono convenzione, accordo generico, partnership, sponsorship</t>
   </si>
   <si>
@@ -111,6 +105,21 @@
   </si>
   <si>
     <t>Qualunque documento, anche di natura tecnica,  pubblicato dall'amministrazione  (e.g., slide, pubblicazioni generiche, rapporti tecnici, documenti di progetto, linee guida diverse da quelle dell'articolo 71 del Codice dell'Amministrazione Digitale)</t>
+  </si>
+  <si>
+    <t>Rientrano in questo concetto tutti i documenti relativi al mero funzionamento interno come per esempio regolamento gestione uffici, note varie attinenti al funzionamento interno dell'ente</t>
+  </si>
+  <si>
+    <t>Rientrano in questo concetto tutte le tipologie di atti normativi quali per esempio la costituzione, il decreto legislativo, il decreto legge, il decreto reale, il regio decreto ma anche regolamento dei contratti, regolamento per i referendum consultiv, ecc.</t>
+  </si>
+  <si>
+    <t>Documento di programmazione e rendicontazione</t>
+  </si>
+  <si>
+    <t>Documenti di programmazione e rendicontazione</t>
+  </si>
+  <si>
+    <t>Rientrano in questo concetto tutte quelle tipologie di documenti relativi alle attività di programmazione e rendicontazione. A titolo d'esempio rientrano documenti quali: bilanci, programma lavori pubblici, documento unico di programmazione, relazione annuale responsbaile anticorruzione, documenti del ciclo della performance, ecc.</t>
   </si>
 </sst>
 </file>
@@ -154,9 +163,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -471,17 +481,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4AA979-1C24-5649-9684-672E16E4105D}">
-  <dimension ref="A1:D9"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="214" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="22.6640625" customWidth="1"/>
-    <col min="2" max="2" width="34.6640625" customWidth="1"/>
-    <col min="3" max="3" width="32.5" customWidth="1"/>
+    <col min="1" max="1" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="43.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="24.5" customWidth="1"/>
   </cols>
   <sheetData>
@@ -510,7 +520,7 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -521,7 +531,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -535,7 +545,7 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -549,7 +559,7 @@
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -563,7 +573,7 @@
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -577,7 +587,7 @@
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -591,7 +601,7 @@
         <v>18</v>
       </c>
       <c r="D8" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -605,7 +615,21 @@
         <v>6</v>
       </c>
       <c r="D9" t="s">
-        <v>25</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C10" t="s">
+        <v>28</v>
+      </c>
+      <c r="D10" t="s">
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
new version 1.0 of IoT ontology with the introduction of new concepts as reported in the owl:versionInfo metadata; correction of typos in l0 ontology
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-documents/government-documents-types/government-documents-types.xlsx
+++ b/VocabolariControllati/classifications-for-documents/government-documents-types/government-documents-types.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/giorgialodi/Desktop/AGID/NuovoDATIGOV/DAF/Git/OntologieVocabolariControllati/VocabolariControllati/classifications-for-documents/government-documents-types/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58BD022B-2132-2F41-AA3D-FEC818248152}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7FDF9AB-A0D7-724F-A3D5-980603760A32}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="15540" xr2:uid="{211D512B-4A7E-2C48-891F-47DA42C0E5D3}"/>
   </bookViews>
@@ -483,8 +483,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF4AA979-1C24-5649-9684-672E16E4105D}">
   <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="214" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="214" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>